<commit_message>
results_PCAcombined_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals werkt! Betere results dan eerst, nu nog de 18 excelletjes
</commit_message>
<xml_diff>
--- a/results_PCAcombined_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
+++ b/results_PCAcombined_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>RMSE_OutSample</t>
+          <t>RMSE_TestSample</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>R2_OutSample</t>
+          <t>R2_TestSample</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Adjusted_R2_OutSample</t>
+          <t>Adjusted_R2_TestSample</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0002560414192102142</v>
+        <v>0.02463865175384928</v>
       </c>
       <c r="C2" t="n">
         <v>0.5970274325464543</v>
@@ -499,16 +499,16 @@
         <v>0.5884169076008656</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3567267652551525</v>
+        <v>0.03543189471917484</v>
       </c>
       <c r="F2" t="n">
-        <v>-123361.9765096056</v>
+        <v>0.9928022233450564</v>
       </c>
       <c r="G2" t="n">
-        <v>-138406.2419376063</v>
+        <v>0.9921357625436728</v>
       </c>
       <c r="H2" t="n">
-        <v>1525.458726246747</v>
+        <v>291.2687803182</v>
       </c>
       <c r="I2" t="n">
         <v>-572.5375606364</v>
@@ -522,7 +522,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0002541058576500429</v>
+        <v>0.01908051223776923</v>
       </c>
       <c r="C3" t="n">
         <v>0.6051076026886225</v>
@@ -531,16 +531,16 @@
         <v>0.5949386997535655</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3567320453670426</v>
+        <v>0.0275803700828647</v>
       </c>
       <c r="F3" t="n">
-        <v>-123365.642734958</v>
+        <v>0.9953448168563664</v>
       </c>
       <c r="G3" t="n">
-        <v>-141870.6391452017</v>
+        <v>0.9948178149910495</v>
       </c>
       <c r="H3" t="n">
-        <v>1526.742017452199</v>
+        <v>346.7694955966112</v>
       </c>
       <c r="I3" t="n">
         <v>-681.5389911932224</v>
@@ -554,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0002527101979916389</v>
+        <v>0.01604666133594783</v>
       </c>
       <c r="C4" t="n">
         <v>0.6128651200966583</v>
@@ -563,16 +563,16 @@
         <v>0.6011843263064712</v>
       </c>
       <c r="E4" t="n">
-        <v>0.356746284989897</v>
+        <v>0.02086707775059352</v>
       </c>
       <c r="F4" t="n">
-        <v>-123375.5104959306</v>
+        <v>0.9974402804563148</v>
       </c>
       <c r="G4" t="n">
-        <v>-145520.0123798156</v>
+        <v>0.9970957028254341</v>
       </c>
       <c r="H4" t="n">
-        <v>1527.846288438371</v>
+        <v>392.133218325583</v>
       </c>
       <c r="I4" t="n">
         <v>-770.266436651166</v>
@@ -586,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0002509331930618039</v>
+        <v>0.0111091205506193</v>
       </c>
       <c r="C5" t="n">
         <v>0.6211481540682555</v>
@@ -595,16 +595,16 @@
         <v>0.6080277438195372</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3567488493612411</v>
+        <v>0.01548468615517097</v>
       </c>
       <c r="F5" t="n">
-        <v>-123377.2838433723</v>
+        <v>0.9984218393605436</v>
       </c>
       <c r="G5" t="n">
-        <v>-149351.6593893454</v>
+        <v>0.9981742847504328</v>
       </c>
       <c r="H5" t="n">
-        <v>1528.432095658451</v>
+        <v>473.0631617584364</v>
       </c>
       <c r="I5" t="n">
         <v>-930.1263235168728</v>
@@ -618,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0002498148031569055</v>
+        <v>0.007475639668471302</v>
       </c>
       <c r="C6" t="n">
         <v>0.6286477389781899</v>
@@ -627,16 +627,16 @@
         <v>0.6141165635469017</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3567505960636795</v>
+        <v>0.01009298211407882</v>
       </c>
       <c r="F6" t="n">
-        <v>-123378.5049206938</v>
+        <v>0.9995341107955057</v>
       </c>
       <c r="G6" t="n">
-        <v>-153389.735847349</v>
+        <v>0.9994502507386968</v>
       </c>
       <c r="H6" t="n">
-        <v>1529.016051953047</v>
+        <v>593.2170164517049</v>
       </c>
       <c r="I6" t="n">
         <v>-1168.43403290341</v>
@@ -650,7 +650,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0002488207394396133</v>
+        <v>0.005785531382205611</v>
       </c>
       <c r="C7" t="n">
         <v>0.6322366064521329</v>
@@ -659,16 +659,16 @@
         <v>0.6161770696159814</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3567486799291574</v>
+        <v>0.00822693784767531</v>
       </c>
       <c r="F7" t="n">
-        <v>-123377.1770221057</v>
+        <v>0.9997546658653153</v>
       </c>
       <c r="G7" t="n">
-        <v>-157648.8928615795</v>
+        <v>0.9997045976745632</v>
       </c>
       <c r="H7" t="n">
-        <v>1530.160293311494</v>
+        <v>718.1476233602531</v>
       </c>
       <c r="I7" t="n">
         <v>-1416.295246720506</v>
@@ -682,7 +682,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0002488207394396133</v>
+        <v>0.005785531382205611</v>
       </c>
       <c r="C8" t="n">
         <v>0.6322366064521329</v>
@@ -691,16 +691,16 @@
         <v>0.6144936357107884</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3567486799291574</v>
+        <v>0.00822693784767531</v>
       </c>
       <c r="F8" t="n">
-        <v>-123377.1770221057</v>
+        <v>0.9997546658653153</v>
       </c>
       <c r="G8" t="n">
-        <v>-162153.1755147675</v>
+        <v>0.99969844345945</v>
       </c>
       <c r="H8" t="n">
-        <v>1530.160293311494</v>
+        <v>718.1476233602531</v>
       </c>
       <c r="I8" t="n">
         <v>-1414.295246720506</v>
@@ -714,7 +714,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0002488207394396133</v>
+        <v>0.005785531382205611</v>
       </c>
       <c r="C9" t="n">
         <v>0.6322366064521329</v>
@@ -723,16 +723,16 @@
         <v>0.6127953697888096</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3567486799291574</v>
+        <v>0.00822693784767531</v>
       </c>
       <c r="F9" t="n">
-        <v>-123377.1770221057</v>
+        <v>0.9997546658653153</v>
       </c>
       <c r="G9" t="n">
-        <v>-166922.4159710842</v>
+        <v>0.9996920273628426</v>
       </c>
       <c r="H9" t="n">
-        <v>1530.160293311494</v>
+        <v>718.1476233602531</v>
       </c>
       <c r="I9" t="n">
         <v>-1412.295246720506</v>

</xml_diff>